<commit_message>
Finished code refactoring, training.py and testing.py now contain the code called by classification.py
</commit_message>
<xml_diff>
--- a/Classification Results/Augmented Data/CORT ONLY VPOP Classification/By Diagnosis/CORT ONLY VPOP Classification Summary.xlsx
+++ b/Classification Results/Augmented Data/CORT ONLY VPOP Classification/By Diagnosis/CORT ONLY VPOP Classification Summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopher/Documents/PTSD/NCDE Model/Classification Results/Augmented Data/CORT ONLY VPOP Classification/By Diagnosis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9CA171-7617-5E49-8B04-F9A313ACC28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F4D505-CF96-2248-B078-99BF97E8B57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19000" yWindow="500" windowWidth="19400" windowHeight="20240" xr2:uid="{064A12D9-DF30-0A45-B172-879C6B680B9E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="16">
   <si>
     <t>Control</t>
   </si>
@@ -81,13 +81,16 @@
   </si>
   <si>
     <t>4, 1, 13, 10</t>
+  </si>
+  <si>
+    <t>Uniform Noise - 1%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -106,6 +109,14 @@
     <font>
       <b/>
       <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -253,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -269,16 +280,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -287,13 +289,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF02A33-AEE7-C74D-B125-3664DD3F27B5}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -621,31 +633,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="18" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="10" t="s">
@@ -657,68 +669,88 @@
         <v>8</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="12"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="4">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+      <c r="E5" s="4">
+        <v>5</v>
+      </c>
       <c r="F5" s="4">
         <f>SUM(C5:E5)/30</f>
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="5">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5">
+        <v>4</v>
+      </c>
       <c r="F6" s="4">
         <f>SUM(C6:E6)/30</f>
-        <v>0</v>
+        <v>0.46666666666666667</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="5">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" s="5">
+        <v>3</v>
+      </c>
       <c r="F7" s="7">
         <f>SUM(C7:E7)/27</f>
-        <v>0</v>
+        <v>0.51851851851851849</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="18"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="7">
         <f>SUM(C5:C7)/29</f>
-        <v>0</v>
+        <v>0.48275862068965519</v>
       </c>
       <c r="D8" s="7">
         <f t="shared" ref="D8:E8" si="0">SUM(D5:D7)/29</f>
-        <v>0</v>
+        <v>0.48275862068965519</v>
       </c>
       <c r="E8" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="7">
+        <v>0.41379310344827586</v>
+      </c>
+      <c r="F8" s="20">
         <f>SUM(C5:E7)/87</f>
-        <v>0</v>
+        <v>0.45977011494252873</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -729,7 +761,7 @@
       </c>
       <c r="F9" s="7">
         <f>SUM(C5:E7)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -740,28 +772,28 @@
       </c>
       <c r="F10" s="7">
         <f>SUM(-F9, 87)</f>
-        <v>87</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
     </row>
     <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="18" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="10" t="s">
@@ -773,68 +805,88 @@
         <v>8</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="12"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="4">
+        <v>4</v>
+      </c>
+      <c r="D14" s="3">
+        <v>5</v>
+      </c>
+      <c r="E14" s="4">
+        <v>5</v>
+      </c>
       <c r="F14" s="4">
         <f>SUM(C14:E14)/30</f>
-        <v>0</v>
+        <v>0.46666666666666667</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="5">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15" s="5">
+        <v>4</v>
+      </c>
       <c r="F15" s="4">
         <f>SUM(C15:E15)/30</f>
-        <v>0</v>
+        <v>0.43333333333333335</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="5">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16" s="5">
+        <v>3</v>
+      </c>
       <c r="F16" s="7">
         <f>SUM(C16:E16)/27</f>
-        <v>0</v>
+        <v>0.48148148148148145</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="18"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="7">
         <f>SUM(C14:C16)/29</f>
-        <v>0</v>
+        <v>0.48275862068965519</v>
       </c>
       <c r="D17" s="7">
         <f t="shared" ref="D17" si="1">SUM(D14:D16)/29</f>
-        <v>0</v>
+        <v>0.48275862068965519</v>
       </c>
       <c r="E17" s="7">
         <f t="shared" ref="E17" si="2">SUM(E14:E16)/29</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="7">
+        <v>0.41379310344827586</v>
+      </c>
+      <c r="F17" s="20">
         <f>SUM(C14:E16)/87</f>
-        <v>0</v>
+        <v>0.45977011494252873</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -845,7 +897,7 @@
       </c>
       <c r="F18" s="7">
         <f>SUM(C14:E16)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -856,35 +908,35 @@
       </c>
       <c r="F19" s="7">
         <f>SUM(-F18, 87)</f>
-        <v>87</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
     </row>
     <row r="22" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="18" t="s">
         <v>11</v>
       </c>
       <c r="F22" s="10" t="s">
@@ -896,16 +948,16 @@
         <v>8</v>
       </c>
       <c r="B23" s="2"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="12"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="16"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="4">
         <v>7</v>
       </c>
@@ -924,7 +976,7 @@
       <c r="A25" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="11"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="5">
         <v>6</v>
       </c>
@@ -943,7 +995,7 @@
       <c r="A26" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="11"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="5">
         <v>5</v>
       </c>
@@ -959,10 +1011,10 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="18"/>
+      <c r="B27" s="15"/>
       <c r="C27" s="7">
         <f>SUM(C24:C26)/29</f>
         <v>0.62068965517241381</v>
@@ -975,7 +1027,7 @@
         <f t="shared" ref="E27" si="4">SUM(E24:E26)/29</f>
         <v>0.65517241379310343</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="20">
         <f>SUM(C24:E26)/87</f>
         <v>0.63218390804597702</v>
       </c>
@@ -1003,24 +1055,24 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
     </row>
     <row r="31" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="E31" s="18" t="s">
         <v>11</v>
       </c>
       <c r="F31" s="10" t="s">
@@ -1032,16 +1084,16 @@
         <v>8</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="12"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="11"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="16"/>
+      <c r="B33" s="13"/>
       <c r="C33" s="4">
         <v>6</v>
       </c>
@@ -1060,7 +1112,7 @@
       <c r="A34" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="11"/>
+      <c r="B34" s="14"/>
       <c r="C34" s="5">
         <v>7</v>
       </c>
@@ -1079,7 +1131,7 @@
       <c r="A35" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="11"/>
+      <c r="B35" s="14"/>
       <c r="C35" s="5">
         <v>6</v>
       </c>
@@ -1095,10 +1147,10 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="18"/>
+      <c r="B36" s="15"/>
       <c r="C36" s="7">
         <f>SUM(C33:C35)/29</f>
         <v>0.65517241379310343</v>
@@ -1111,7 +1163,7 @@
         <f t="shared" ref="E36" si="6">SUM(E33:E35)/29</f>
         <v>0.65517241379310343</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="20">
         <f>SUM(C33:E35)/87</f>
         <v>0.65517241379310343</v>
       </c>
@@ -1138,35 +1190,266 @@
         <v>30</v>
       </c>
     </row>
+    <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+    </row>
+    <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+    </row>
+    <row r="41" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="11"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="13"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4">
+        <f>SUM(C43:E43)/30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="14"/>
+      <c r="C44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="4">
+        <f>SUM(C44:E44)/30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" s="14"/>
+      <c r="C45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="7">
+        <f>SUM(C45:E45)/27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="15"/>
+      <c r="C46" s="7">
+        <f>SUM(C43:C45)/29</f>
+        <v>0</v>
+      </c>
+      <c r="D46" s="7">
+        <f t="shared" ref="D46:E46" si="7">SUM(D43:D45)/29</f>
+        <v>0</v>
+      </c>
+      <c r="E46" s="7">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F46" s="20">
+        <f>SUM(C43:E45)/87</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
+      <c r="E47" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" s="7">
+        <f>SUM(C43:E45)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="E48" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="7">
+        <f>SUM(-F47, 87)</f>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A49" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
+    </row>
+    <row r="50" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="11"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="13"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4">
+        <f>SUM(C52:E52)/30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="14"/>
+      <c r="C53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="4">
+        <f>SUM(C53:E53)/30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" s="14"/>
+      <c r="C54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="7">
+        <f>SUM(C54:E54)/27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55" s="15"/>
+      <c r="C55" s="7">
+        <f>SUM(C52:C54)/29</f>
+        <v>0</v>
+      </c>
+      <c r="D55" s="7">
+        <f t="shared" ref="D55:E55" si="8">SUM(D52:D54)/29</f>
+        <v>0</v>
+      </c>
+      <c r="E55" s="7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="20">
+        <f>SUM(C52:E54)/87</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
+      <c r="E56" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F56" s="7">
+        <f>SUM(C52:E54)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="8"/>
+      <c r="B57" s="8"/>
+      <c r="E57" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F57" s="7">
+        <f>SUM(-F56, 87)</f>
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="A14:B14"/>
+  <mergeCells count="56">
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A2:C2"/>
@@ -1177,6 +1460,33 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>